<commit_message>
nova função pra testar se mse vt é o melhor msm
</commit_message>
<xml_diff>
--- a/function_ensemble/redes-ensemble-s/Teste01/content/results/metrics_20_1.xlsx
+++ b/function_ensemble/redes-ensemble-s/Teste01/content/results/metrics_20_1.xlsx
@@ -522,52 +522,52 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.9995105437032389</v>
+        <v>0.995378733760833</v>
       </c>
       <c r="C2" t="n">
-        <v>-0.5764249449502077</v>
+        <v>0.7119947686249386</v>
       </c>
       <c r="D2" t="n">
-        <v>0.9993986693798166</v>
+        <v>0.9939346300715752</v>
       </c>
       <c r="E2" t="n">
-        <v>0.9921314997151127</v>
+        <v>0.985405948427343</v>
       </c>
       <c r="F2" t="n">
-        <v>0.9988816303394024</v>
+        <v>0.9926861151235654</v>
       </c>
       <c r="G2" t="n">
-        <v>0.0723808123593857</v>
+        <v>0.002743383267876626</v>
       </c>
       <c r="H2" t="n">
-        <v>233.1217697966957</v>
+        <v>0.1709723465224299</v>
       </c>
       <c r="I2" t="n">
-        <v>0.01066154088254835</v>
+        <v>0.003658611867849484</v>
       </c>
       <c r="J2" t="n">
-        <v>0.01207208315876411</v>
+        <v>0.003210421913200622</v>
       </c>
       <c r="K2" t="n">
-        <v>0.01136681202065623</v>
+        <v>0.003434516890525053</v>
       </c>
       <c r="L2" t="n">
-        <v>0.05360490967818426</v>
+        <v>0.03007855280777443</v>
       </c>
       <c r="M2" t="n">
-        <v>0.269036823426433</v>
+        <v>0.05237731634855518</v>
       </c>
       <c r="N2" t="n">
-        <v>1.00090361162479</v>
+        <v>1.008531568441539</v>
       </c>
       <c r="O2" t="n">
-        <v>0.2804902779826968</v>
+        <v>0.05460712714150513</v>
       </c>
       <c r="P2" t="n">
-        <v>79.2516280747512</v>
+        <v>85.79712670196956</v>
       </c>
       <c r="Q2" t="n">
-        <v>124.3500335948746</v>
+        <v>130.895532222093</v>
       </c>
     </row>
     <row r="3">
@@ -577,52 +577,52 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.9996030657374066</v>
+        <v>0.9962339467912211</v>
       </c>
       <c r="C3" t="n">
-        <v>-0.579697624685185</v>
+        <v>0.7111629443048144</v>
       </c>
       <c r="D3" t="n">
-        <v>0.9995015903195894</v>
+        <v>0.9948323626179923</v>
       </c>
       <c r="E3" t="n">
-        <v>0.9936440122835237</v>
+        <v>0.9883715256082389</v>
       </c>
       <c r="F3" t="n">
-        <v>0.9990855573817748</v>
+        <v>0.9939573147153939</v>
       </c>
       <c r="G3" t="n">
-        <v>0.05869865107445976</v>
+        <v>0.002235691869758906</v>
       </c>
       <c r="H3" t="n">
-        <v>233.605733777499</v>
+        <v>0.1714661533717953</v>
       </c>
       <c r="I3" t="n">
-        <v>0.008836761351575682</v>
+        <v>0.003117102448434861</v>
       </c>
       <c r="J3" t="n">
-        <v>0.009751542160677999</v>
+        <v>0.002558049683361868</v>
       </c>
       <c r="K3" t="n">
-        <v>0.009294151756126842</v>
+        <v>0.002837576065898365</v>
       </c>
       <c r="L3" t="n">
-        <v>0.0483757304516161</v>
+        <v>0.02701397453362797</v>
       </c>
       <c r="M3" t="n">
-        <v>0.2422780449699472</v>
+        <v>0.04728310342774579</v>
       </c>
       <c r="N3" t="n">
-        <v>1.000732801715557</v>
+        <v>1.006952713616207</v>
       </c>
       <c r="O3" t="n">
-        <v>0.2525923229290107</v>
+        <v>0.04929604303018238</v>
       </c>
       <c r="P3" t="n">
-        <v>79.6706770648086</v>
+        <v>86.20640907481494</v>
       </c>
       <c r="Q3" t="n">
-        <v>124.769082584932</v>
+        <v>131.3048145949384</v>
       </c>
     </row>
     <row r="4">
@@ -632,52 +632,52 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.9996781000471054</v>
+        <v>0.9969168718341714</v>
       </c>
       <c r="C4" t="n">
-        <v>-0.5826537453191345</v>
+        <v>0.7104213363562253</v>
       </c>
       <c r="D4" t="n">
-        <v>0.999586625317481</v>
+        <v>0.9955361278286112</v>
       </c>
       <c r="E4" t="n">
-        <v>0.9948572088628785</v>
+        <v>0.9907141151188346</v>
       </c>
       <c r="F4" t="n">
-        <v>0.9992512845234589</v>
+        <v>0.9949580155432958</v>
       </c>
       <c r="G4" t="n">
-        <v>0.04760257502689241</v>
+        <v>0.001830278063437788</v>
       </c>
       <c r="H4" t="n">
-        <v>234.0428849886152</v>
+        <v>0.1719064038858731</v>
       </c>
       <c r="I4" t="n">
-        <v>0.007329098052819944</v>
+        <v>0.002692593509634036</v>
       </c>
       <c r="J4" t="n">
-        <v>0.007890220502975283</v>
+        <v>0.002042723239501642</v>
       </c>
       <c r="K4" t="n">
-        <v>0.00760974513047013</v>
+        <v>0.002367658374567839</v>
       </c>
       <c r="L4" t="n">
-        <v>0.04383582008495665</v>
+        <v>0.02425486584534641</v>
       </c>
       <c r="M4" t="n">
-        <v>0.2181801435211106</v>
+        <v>0.04278174918628021</v>
       </c>
       <c r="N4" t="n">
-        <v>1.000594276836113</v>
+        <v>1.00569192892153</v>
       </c>
       <c r="O4" t="n">
-        <v>0.2274685239259642</v>
+        <v>0.04460305681956977</v>
       </c>
       <c r="P4" t="n">
-        <v>80.08973684400868</v>
+        <v>86.60657475287572</v>
       </c>
       <c r="Q4" t="n">
-        <v>125.1881423641321</v>
+        <v>131.7049802729991</v>
       </c>
     </row>
     <row r="5">
@@ -687,52 +687,52 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.9997389516659273</v>
+        <v>0.9974616137848186</v>
       </c>
       <c r="C5" t="n">
-        <v>-0.5853226897509585</v>
+        <v>0.7097609290954167</v>
       </c>
       <c r="D5" t="n">
-        <v>0.9996569765333813</v>
+        <v>0.9960847015465237</v>
       </c>
       <c r="E5" t="n">
-        <v>0.9958336663524147</v>
+        <v>0.9925553348333443</v>
       </c>
       <c r="F5" t="n">
-        <v>0.9993863531091532</v>
+        <v>0.9957416081212127</v>
       </c>
       <c r="G5" t="n">
-        <v>0.03860383574647219</v>
+        <v>0.00150689570990667</v>
       </c>
       <c r="H5" t="n">
-        <v>234.4375685740462</v>
+        <v>0.1722984501639973</v>
       </c>
       <c r="I5" t="n">
-        <v>0.006081776963084553</v>
+        <v>0.00236169558610606</v>
       </c>
       <c r="J5" t="n">
-        <v>0.006392110877521288</v>
+        <v>0.001637688894580317</v>
       </c>
       <c r="K5" t="n">
-        <v>0.006236943920302921</v>
+        <v>0.001999692240343188</v>
       </c>
       <c r="L5" t="n">
-        <v>0.03973257241356786</v>
+        <v>0.02197647192410817</v>
       </c>
       <c r="M5" t="n">
-        <v>0.1964785885191366</v>
+        <v>0.03881875461560649</v>
       </c>
       <c r="N5" t="n">
-        <v>1.00048193538598</v>
+        <v>1.004686251474181</v>
       </c>
       <c r="O5" t="n">
-        <v>0.2048430887991443</v>
+        <v>0.04047134936549276</v>
       </c>
       <c r="P5" t="n">
-        <v>80.50880727155625</v>
+        <v>86.99540713102078</v>
       </c>
       <c r="Q5" t="n">
-        <v>125.6072127916797</v>
+        <v>132.0938126511442</v>
       </c>
     </row>
     <row r="6">
@@ -742,52 +742,52 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.9997883010342775</v>
+        <v>0.9978956056807017</v>
       </c>
       <c r="C6" t="n">
-        <v>-0.5877313641575499</v>
+        <v>0.7091667716187772</v>
       </c>
       <c r="D6" t="n">
-        <v>0.9997152327343759</v>
+        <v>0.9965098981800566</v>
       </c>
       <c r="E6" t="n">
-        <v>0.9966208735694808</v>
+        <v>0.9939941487290305</v>
       </c>
       <c r="F6" t="n">
-        <v>0.9994965800086383</v>
+        <v>0.9963517057297677</v>
       </c>
       <c r="G6" t="n">
-        <v>0.03130604962287221</v>
+        <v>0.001249259373036695</v>
       </c>
       <c r="H6" t="n">
-        <v>234.7937634200662</v>
+        <v>0.1726511677083971</v>
       </c>
       <c r="I6" t="n">
-        <v>0.005048899461558088</v>
+        <v>0.002105218327839763</v>
       </c>
       <c r="J6" t="n">
-        <v>0.005184354552487615</v>
+        <v>0.001321176400655552</v>
       </c>
       <c r="K6" t="n">
-        <v>0.005116627007022851</v>
+        <v>0.001713197364247658</v>
       </c>
       <c r="L6" t="n">
-        <v>0.03601582418885826</v>
+        <v>0.01992641316972057</v>
       </c>
       <c r="M6" t="n">
-        <v>0.1769351565485848</v>
+        <v>0.03534486346043361</v>
       </c>
       <c r="N6" t="n">
-        <v>1.000390828859795</v>
+        <v>1.003885035666397</v>
       </c>
       <c r="O6" t="n">
-        <v>0.1844676524691248</v>
+        <v>0.03684956747189813</v>
       </c>
       <c r="P6" t="n">
-        <v>80.92788784285187</v>
+        <v>87.37040880967399</v>
       </c>
       <c r="Q6" t="n">
-        <v>126.0262933629753</v>
+        <v>132.4688143297974</v>
       </c>
     </row>
     <row r="7">
@@ -797,52 +797,52 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.9998283172613143</v>
+        <v>0.9982407361500495</v>
       </c>
       <c r="C7" t="n">
-        <v>-0.5899046875756211</v>
+        <v>0.7086267098735354</v>
       </c>
       <c r="D7" t="n">
-        <v>0.9997634585563864</v>
+        <v>0.9968374207468499</v>
       </c>
       <c r="E7" t="n">
-        <v>0.9972573688243829</v>
+        <v>0.9951095100602375</v>
       </c>
       <c r="F7" t="n">
-        <v>0.999586683179154</v>
+        <v>0.9968233094715906</v>
       </c>
       <c r="G7" t="n">
-        <v>0.02538844872644399</v>
+        <v>0.001044375017571852</v>
       </c>
       <c r="H7" t="n">
-        <v>235.1151545545977</v>
+        <v>0.1729717716898253</v>
       </c>
       <c r="I7" t="n">
-        <v>0.004193859728505041</v>
+        <v>0.001907657756267259</v>
       </c>
       <c r="J7" t="n">
-        <v>0.004207824925603744</v>
+        <v>0.001075817499392466</v>
       </c>
       <c r="K7" t="n">
-        <v>0.004200842327054393</v>
+        <v>0.001491737627829862</v>
       </c>
       <c r="L7" t="n">
-        <v>0.03265045462453933</v>
+        <v>0.01816050569090145</v>
       </c>
       <c r="M7" t="n">
-        <v>0.1593375308156995</v>
+        <v>0.03231679157298652</v>
       </c>
       <c r="N7" t="n">
-        <v>1.000316952748343</v>
+        <v>1.003247871722986</v>
       </c>
       <c r="O7" t="n">
-        <v>0.1661208593766834</v>
+        <v>0.03369258429522948</v>
       </c>
       <c r="P7" t="n">
-        <v>81.34692196589681</v>
+        <v>87.72867328357877</v>
       </c>
       <c r="Q7" t="n">
-        <v>126.4453274860202</v>
+        <v>132.8270788037022</v>
       </c>
     </row>
     <row r="8">
@@ -852,52 +852,52 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.9998607694852849</v>
+        <v>0.9985146861029791</v>
       </c>
       <c r="C8" t="n">
-        <v>-0.5918644066398784</v>
+        <v>0.7081287461828661</v>
       </c>
       <c r="D8" t="n">
-        <v>0.9998034562785859</v>
+        <v>0.9970879852004207</v>
       </c>
       <c r="E8" t="n">
-        <v>0.9977714037860154</v>
+        <v>0.9959659214659383</v>
       </c>
       <c r="F8" t="n">
-        <v>0.9996603669084809</v>
+        <v>0.9971848327149049</v>
       </c>
       <c r="G8" t="n">
-        <v>0.02058941283824998</v>
+        <v>0.000881746491491093</v>
       </c>
       <c r="H8" t="n">
-        <v>235.4049578706563</v>
+        <v>0.1732673844475179</v>
       </c>
       <c r="I8" t="n">
-        <v>0.003484703507074101</v>
+        <v>0.001756518074052746</v>
       </c>
       <c r="J8" t="n">
-        <v>0.003419177460564085</v>
+        <v>0.0008874228010533075</v>
       </c>
       <c r="K8" t="n">
-        <v>0.003451940483819093</v>
+        <v>0.001321970437553027</v>
       </c>
       <c r="L8" t="n">
-        <v>0.02959856600818865</v>
+        <v>0.01663907405272054</v>
       </c>
       <c r="M8" t="n">
-        <v>0.1434901140784618</v>
+        <v>0.0296942164653505</v>
       </c>
       <c r="N8" t="n">
-        <v>1.000257040950243</v>
+        <v>1.002742117963731</v>
       </c>
       <c r="O8" t="n">
-        <v>0.1495987853002664</v>
+        <v>0.03095836073578251</v>
       </c>
       <c r="P8" t="n">
-        <v>81.7659565503795</v>
+        <v>88.06721193577026</v>
       </c>
       <c r="Q8" t="n">
-        <v>126.8643620705029</v>
+        <v>133.1656174558937</v>
       </c>
     </row>
     <row r="9">
@@ -907,52 +907,52 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.999887088817274</v>
+        <v>0.9987316342519548</v>
       </c>
       <c r="C9" t="n">
-        <v>-0.5936320082581363</v>
+        <v>0.7076659377075043</v>
       </c>
       <c r="D9" t="n">
-        <v>0.9998365868787142</v>
+        <v>0.9972782310939691</v>
       </c>
       <c r="E9" t="n">
-        <v>0.9981887181780775</v>
+        <v>0.9966159136558261</v>
       </c>
       <c r="F9" t="n">
-        <v>0.9997207609841001</v>
+        <v>0.9974592665548651</v>
       </c>
       <c r="G9" t="n">
-        <v>0.01669730920666731</v>
+        <v>0.0007529566985870966</v>
       </c>
       <c r="H9" t="n">
-        <v>235.6663508528365</v>
+        <v>0.1735421275507779</v>
       </c>
       <c r="I9" t="n">
-        <v>0.002897300777402213</v>
+        <v>0.00164176235557897</v>
       </c>
       <c r="J9" t="n">
-        <v>0.002778921520814192</v>
+        <v>0.0007444365193181759</v>
       </c>
       <c r="K9" t="n">
-        <v>0.002838111149108202</v>
+        <v>0.001193099437448573</v>
       </c>
       <c r="L9" t="n">
-        <v>0.026832146356434</v>
+        <v>0.01526842679958859</v>
       </c>
       <c r="M9" t="n">
-        <v>0.1292180684218245</v>
+        <v>0.02744005646107706</v>
       </c>
       <c r="N9" t="n">
-        <v>1.000208451414264</v>
+        <v>1.002341598304084</v>
       </c>
       <c r="O9" t="n">
-        <v>0.1347191491128186</v>
+        <v>0.02860823647337266</v>
       </c>
       <c r="P9" t="n">
-        <v>82.18501539578155</v>
+        <v>88.38300567402857</v>
       </c>
       <c r="Q9" t="n">
-        <v>127.283420915905</v>
+        <v>133.481411194152</v>
       </c>
     </row>
     <row r="10">
@@ -962,52 +962,52 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.9999084268991874</v>
+        <v>0.998902924083356</v>
       </c>
       <c r="C10" t="n">
-        <v>-0.5952234986908682</v>
+        <v>0.707232612349755</v>
       </c>
       <c r="D10" t="n">
-        <v>0.9998641507313899</v>
+        <v>0.997421425735956</v>
       </c>
       <c r="E10" t="n">
-        <v>0.9985252290103349</v>
+        <v>0.9971009093489795</v>
       </c>
       <c r="F10" t="n">
-        <v>0.999770200958684</v>
+        <v>0.9976648344237579</v>
       </c>
       <c r="G10" t="n">
-        <v>0.0135418329909129</v>
+        <v>0.000651271655331833</v>
       </c>
       <c r="H10" t="n">
-        <v>235.901700507434</v>
+        <v>0.1737993682018187</v>
       </c>
       <c r="I10" t="n">
-        <v>0.002408596007815299</v>
+        <v>0.001555387802539629</v>
       </c>
       <c r="J10" t="n">
-        <v>0.002262636764665809</v>
+        <v>0.000637746420728643</v>
       </c>
       <c r="K10" t="n">
-        <v>0.002335616386240554</v>
+        <v>0.001096567111634136</v>
       </c>
       <c r="L10" t="n">
-        <v>0.02432270913720351</v>
+        <v>0.01403413426156044</v>
       </c>
       <c r="M10" t="n">
-        <v>0.1163693816728133</v>
+        <v>0.02552002459504757</v>
       </c>
       <c r="N10" t="n">
-        <v>1.00016905803227</v>
+        <v>1.002025370923035</v>
       </c>
       <c r="O10" t="n">
-        <v>0.1213234671684538</v>
+        <v>0.02660646487579241</v>
       </c>
       <c r="P10" t="n">
-        <v>82.6039432893398</v>
+        <v>88.67316742700092</v>
       </c>
       <c r="Q10" t="n">
-        <v>127.7023488094632</v>
+        <v>133.7715729471244</v>
       </c>
     </row>
     <row r="11">
@@ -1017,52 +1017,52 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0.9999257322366716</v>
+        <v>0.9990377322396815</v>
       </c>
       <c r="C11" t="n">
-        <v>-0.5966583337302918</v>
+        <v>0.7068264317036361</v>
       </c>
       <c r="D11" t="n">
-        <v>0.9998869792618724</v>
+        <v>0.9975279672717687</v>
       </c>
       <c r="E11" t="n">
-        <v>0.9987991857872952</v>
+        <v>0.9974554324354431</v>
       </c>
       <c r="F11" t="n">
-        <v>0.9998107894070137</v>
+        <v>0.9978163011039608</v>
       </c>
       <c r="G11" t="n">
-        <v>0.01098271914653187</v>
+        <v>0.0005712437103279199</v>
       </c>
       <c r="H11" t="n">
-        <v>236.113883957606</v>
+        <v>0.1740404945794451</v>
       </c>
       <c r="I11" t="n">
-        <v>0.002003848098995894</v>
+        <v>0.001491122286677756</v>
       </c>
       <c r="J11" t="n">
-        <v>0.001842324268811423</v>
+        <v>0.0005597578868488029</v>
       </c>
       <c r="K11" t="n">
-        <v>0.001923086183903658</v>
+        <v>0.001025440086763279</v>
       </c>
       <c r="L11" t="n">
-        <v>0.02204854658277559</v>
+        <v>0.01292263891435626</v>
       </c>
       <c r="M11" t="n">
-        <v>0.1047984691993727</v>
+        <v>0.02390070522658107</v>
       </c>
       <c r="N11" t="n">
-        <v>1.000137109716914</v>
+        <v>1.001776494326742</v>
       </c>
       <c r="O11" t="n">
-        <v>0.109259956995928</v>
+        <v>0.02491820772935708</v>
       </c>
       <c r="P11" t="n">
-        <v>83.02286445631236</v>
+        <v>88.9353892523667</v>
       </c>
       <c r="Q11" t="n">
-        <v>128.1212699764358</v>
+        <v>134.0337947724901</v>
       </c>
     </row>
     <row r="12">
@@ -1072,52 +1072,52 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>0.9999397691147613</v>
+        <v>0.9991434367008153</v>
       </c>
       <c r="C12" t="n">
-        <v>-0.5979511838667271</v>
+        <v>0.7064457944941227</v>
       </c>
       <c r="D12" t="n">
-        <v>0.999906014523557</v>
+        <v>0.9976061258810635</v>
       </c>
       <c r="E12" t="n">
-        <v>0.9990226996406153</v>
+        <v>0.9977076966319774</v>
       </c>
       <c r="F12" t="n">
-        <v>0.9998442620975654</v>
+        <v>0.9979255866496723</v>
       </c>
       <c r="G12" t="n">
-        <v>0.008906945178852224</v>
+        <v>0.0005084929760039369</v>
       </c>
       <c r="H12" t="n">
-        <v>236.3050706759164</v>
+        <v>0.1742664572696835</v>
       </c>
       <c r="I12" t="n">
-        <v>0.001666354524167056</v>
+        <v>0.001443977261903559</v>
       </c>
       <c r="J12" t="n">
-        <v>0.001499402781015678</v>
+        <v>0.000504264420867977</v>
       </c>
       <c r="K12" t="n">
-        <v>0.001582878652591367</v>
+        <v>0.000974120841385768</v>
       </c>
       <c r="L12" t="n">
-        <v>0.01997394764206466</v>
+        <v>0.01192170611937634</v>
       </c>
       <c r="M12" t="n">
-        <v>0.09437661351654987</v>
+        <v>0.02254978882393218</v>
       </c>
       <c r="N12" t="n">
-        <v>1.000111195480441</v>
+        <v>1.001581347629264</v>
       </c>
       <c r="O12" t="n">
-        <v>0.09839442134047199</v>
+        <v>0.02350978001866496</v>
       </c>
       <c r="P12" t="n">
-        <v>83.44184789877997</v>
+        <v>89.16811831147865</v>
       </c>
       <c r="Q12" t="n">
-        <v>128.5402534189034</v>
+        <v>134.2665238316021</v>
       </c>
     </row>
     <row r="13">
@@ -1127,52 +1127,52 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>0.9999511474027314</v>
+        <v>0.9992259437245948</v>
       </c>
       <c r="C13" t="n">
-        <v>-0.5991151809854485</v>
+        <v>0.7060893896608844</v>
       </c>
       <c r="D13" t="n">
-        <v>0.9999217882489148</v>
+        <v>0.9976624120238153</v>
       </c>
       <c r="E13" t="n">
-        <v>0.9992035675644766</v>
+        <v>0.9978798625850107</v>
       </c>
       <c r="F13" t="n">
-        <v>0.9998716699813025</v>
+        <v>0.9980020631176624</v>
       </c>
       <c r="G13" t="n">
-        <v>0.00722432360062459</v>
+        <v>0.0004595132425705223</v>
       </c>
       <c r="H13" t="n">
-        <v>236.4772026059673</v>
+        <v>0.174478034574581</v>
       </c>
       <c r="I13" t="n">
-        <v>0.001386687711723489</v>
+        <v>0.001410025639447276</v>
       </c>
       <c r="J13" t="n">
-        <v>0.00122190992487373</v>
+        <v>0.000466391089697857</v>
       </c>
       <c r="K13" t="n">
-        <v>0.001304312206003889</v>
+        <v>0.0009382083645725666</v>
       </c>
       <c r="L13" t="n">
-        <v>0.01809969662494014</v>
+        <v>0.01102049282363301</v>
       </c>
       <c r="M13" t="n">
-        <v>0.08499602108701672</v>
+        <v>0.02143625999493667</v>
       </c>
       <c r="N13" t="n">
-        <v>1.000090189410342</v>
+        <v>1.001429026969979</v>
       </c>
       <c r="O13" t="n">
-        <v>0.0886144776707103</v>
+        <v>0.02234884596209666</v>
       </c>
       <c r="P13" t="n">
-        <v>83.86060333731383</v>
+        <v>89.3706855941229</v>
       </c>
       <c r="Q13" t="n">
-        <v>128.9590088574373</v>
+        <v>134.4690911142463</v>
       </c>
     </row>
     <row r="14">
@@ -1182,52 +1182,52 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0.999960381876084</v>
+        <v>0.9992899748462839</v>
       </c>
       <c r="C14" t="n">
-        <v>-0.6001619857082197</v>
+        <v>0.7057556453850695</v>
       </c>
       <c r="D14" t="n">
-        <v>0.9999350073826545</v>
+        <v>0.9977019193881276</v>
       </c>
       <c r="E14" t="n">
-        <v>0.9993501881359377</v>
+        <v>0.9979895928337482</v>
       </c>
       <c r="F14" t="n">
-        <v>0.9998942675055457</v>
+        <v>0.9980531390450642</v>
       </c>
       <c r="G14" t="n">
-        <v>0.005858729394566502</v>
+        <v>0.0004215016027354626</v>
       </c>
       <c r="H14" t="n">
-        <v>236.632004120867</v>
+        <v>0.1746761595937067</v>
       </c>
       <c r="I14" t="n">
-        <v>0.001152313591949233</v>
+        <v>0.001386194922830489</v>
       </c>
       <c r="J14" t="n">
-        <v>0.0009969603579450884</v>
+        <v>0.0004422524607959401</v>
       </c>
       <c r="K14" t="n">
-        <v>0.001074636974947161</v>
+        <v>0.0009142236918132144</v>
       </c>
       <c r="L14" t="n">
-        <v>0.01638500363948702</v>
+        <v>0.0102092929335801</v>
       </c>
       <c r="M14" t="n">
-        <v>0.07654233726877238</v>
+        <v>0.02053050420071223</v>
       </c>
       <c r="N14" t="n">
-        <v>1.000073141151845</v>
+        <v>1.001310815668399</v>
       </c>
       <c r="O14" t="n">
-        <v>0.07980090303078535</v>
+        <v>0.02140453026853912</v>
       </c>
       <c r="P14" t="n">
-        <v>84.27964505153869</v>
+        <v>89.54337395614596</v>
       </c>
       <c r="Q14" t="n">
-        <v>129.3780505716621</v>
+        <v>134.6417794762694</v>
       </c>
     </row>
     <row r="15">
@@ -1237,52 +1237,52 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>0.9999999811938003</v>
+        <v>0.9993393581354908</v>
       </c>
       <c r="C15" t="n">
-        <v>-0.6094485551652917</v>
+        <v>0.7054448202389667</v>
       </c>
       <c r="D15" t="n">
-        <v>0.9999998645306705</v>
+        <v>0.9977285321265024</v>
       </c>
       <c r="E15" t="n">
-        <v>0.9999989695861782</v>
+        <v>0.9980519298567855</v>
       </c>
       <c r="F15" t="n">
-        <v>0.9999998040705005</v>
+        <v>0.9980848324401307</v>
       </c>
       <c r="G15" t="n">
-        <v>2.781061393531285e-06</v>
+        <v>0.0003921855490152145</v>
       </c>
       <c r="H15" t="n">
-        <v>238.0053023004647</v>
+        <v>0.1748606788273805</v>
       </c>
       <c r="I15" t="n">
-        <v>2.401859720325587e-06</v>
+        <v>0.001370142203606005</v>
       </c>
       <c r="J15" t="n">
-        <v>1.580891007787593e-06</v>
+        <v>0.0004285394665827599</v>
       </c>
       <c r="K15" t="n">
-        <v>1.99137536405659e-06</v>
+        <v>0.0008993408350943826</v>
       </c>
       <c r="L15" t="n">
-        <v>0.0007331383749497421</v>
+        <v>0.009478878060547959</v>
       </c>
       <c r="M15" t="n">
-        <v>0.001667651460447082</v>
+        <v>0.01980367513910523</v>
       </c>
       <c r="N15" t="n">
-        <v>1.000000034719138</v>
+        <v>1.001219646519094</v>
       </c>
       <c r="O15" t="n">
-        <v>0.001738646835632741</v>
+        <v>0.02064675858903593</v>
       </c>
       <c r="P15" t="n">
-        <v>99.58535581378618</v>
+        <v>89.68755098167802</v>
       </c>
       <c r="Q15" t="n">
-        <v>144.6837613339096</v>
+        <v>134.7859565018014</v>
       </c>
     </row>
     <row r="16">
@@ -1292,52 +1292,52 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>0.9999999993392285</v>
+        <v>0.9993771273140193</v>
       </c>
       <c r="C16" t="n">
-        <v>-0.6096134835969966</v>
+        <v>0.7051555362230676</v>
       </c>
       <c r="D16" t="n">
-        <v>0.9999999886540967</v>
+        <v>0.9977454306759094</v>
       </c>
       <c r="E16" t="n">
-        <v>0.9999999620379838</v>
+        <v>0.9980779865561885</v>
       </c>
       <c r="F16" t="n">
-        <v>0.9999999872387287</v>
+        <v>0.9981017889254901</v>
       </c>
       <c r="G16" t="n">
-        <v>9.771491331053915e-08</v>
+        <v>0.0003697641330972075</v>
       </c>
       <c r="H16" t="n">
-        <v>238.0296919220652</v>
+        <v>0.175032410315637</v>
       </c>
       <c r="I16" t="n">
-        <v>2.011619034924323e-07</v>
+        <v>0.001359949052299538</v>
       </c>
       <c r="J16" t="n">
-        <v>5.824243504532769e-08</v>
+        <v>0.0004228074737682526</v>
       </c>
       <c r="K16" t="n">
-        <v>1.2970216926888e-07</v>
+        <v>0.0008913782630338951</v>
       </c>
       <c r="L16" t="n">
-        <v>0.0001704113783639889</v>
+        <v>0.0088214104407363</v>
       </c>
       <c r="M16" t="n">
-        <v>0.0003125938472051859</v>
+        <v>0.01922925201606156</v>
       </c>
       <c r="N16" t="n">
-        <v>1.000000001219886</v>
+        <v>1.001149918804888</v>
       </c>
       <c r="O16" t="n">
-        <v>0.0003259016144391805</v>
+        <v>0.0200478810844245</v>
       </c>
       <c r="P16" t="n">
-        <v>106.2824232912622</v>
+        <v>89.80529046743445</v>
       </c>
       <c r="Q16" t="n">
-        <v>151.3808288113857</v>
+        <v>134.9036959875579</v>
       </c>
     </row>
     <row r="17">
@@ -1347,52 +1347,52 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>0.9999999996864509</v>
+        <v>0.9994057183510918</v>
       </c>
       <c r="C17" t="n">
-        <v>-0.6096315700007242</v>
+        <v>0.7048873443815674</v>
       </c>
       <c r="D17" t="n">
-        <v>0.9999999939834622</v>
+        <v>0.9977549626361173</v>
       </c>
       <c r="E17" t="n">
-        <v>0.9999999178684058</v>
+        <v>0.998077113341287</v>
       </c>
       <c r="F17" t="n">
-        <v>0.9999999885533509</v>
+        <v>0.9981077063999175</v>
       </c>
       <c r="G17" t="n">
-        <v>4.636765083890706e-08</v>
+        <v>0.0003527912584224518</v>
       </c>
       <c r="H17" t="n">
-        <v>238.0323665400098</v>
+        <v>0.1751916205780359</v>
       </c>
       <c r="I17" t="n">
-        <v>1.066727045529373e-07</v>
+        <v>0.001354199404190353</v>
       </c>
       <c r="J17" t="n">
-        <v>1.260086927712851e-07</v>
+        <v>0.0004229995649254357</v>
       </c>
       <c r="K17" t="n">
-        <v>1.163406986621112e-07</v>
+        <v>0.0008885994845578941</v>
       </c>
       <c r="L17" t="n">
-        <v>0.0001216133866130939</v>
+        <v>0.008258888533213746</v>
       </c>
       <c r="M17" t="n">
-        <v>0.0002153314905881326</v>
+        <v>0.01878273831001358</v>
       </c>
       <c r="N17" t="n">
-        <v>1.00000000057886</v>
+        <v>1.001097135351831</v>
       </c>
       <c r="O17" t="n">
-        <v>0.0002244985979401049</v>
+        <v>0.01958235836549926</v>
       </c>
       <c r="P17" t="n">
-        <v>107.7733276021066</v>
+        <v>89.8992680237055</v>
       </c>
       <c r="Q17" t="n">
-        <v>152.87173312223</v>
+        <v>134.9976735438289</v>
       </c>
     </row>
     <row r="18">
@@ -1402,52 +1402,52 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>0.9999999997629182</v>
+        <v>0.9994271084877091</v>
       </c>
       <c r="C18" t="n">
-        <v>-0.6096389565638431</v>
+        <v>0.7046397068756509</v>
       </c>
       <c r="D18" t="n">
-        <v>0.999999996350974</v>
+        <v>0.9977590204498158</v>
       </c>
       <c r="E18" t="n">
-        <v>0.9999999003775992</v>
+        <v>0.9980566998916318</v>
       </c>
       <c r="F18" t="n">
-        <v>0.9999999892981991</v>
+        <v>0.998105531174873</v>
       </c>
       <c r="G18" t="n">
-        <v>3.505965994382825e-08</v>
+        <v>0.0003400931493206264</v>
       </c>
       <c r="H18" t="n">
-        <v>238.0334588651932</v>
+        <v>0.1753386288989311</v>
       </c>
       <c r="I18" t="n">
-        <v>6.469692111507101e-08</v>
+        <v>0.001351751743861323</v>
       </c>
       <c r="J18" t="n">
-        <v>1.5284359946659e-07</v>
+        <v>0.0004274901469801044</v>
       </c>
       <c r="K18" t="n">
-        <v>1.087702602908305e-07</v>
+        <v>0.0008896209454207137</v>
       </c>
       <c r="L18" t="n">
-        <v>0.0001009418757217764</v>
+        <v>0.007758616959256229</v>
       </c>
       <c r="M18" t="n">
-        <v>0.0001872422493558231</v>
+        <v>0.01844161460720363</v>
       </c>
       <c r="N18" t="n">
-        <v>1.000000000437689</v>
+        <v>1.001057645868845</v>
       </c>
       <c r="O18" t="n">
-        <v>0.0001952135395557907</v>
+        <v>0.01922671232043728</v>
       </c>
       <c r="P18" t="n">
-        <v>108.3324293135273</v>
+        <v>89.97258201857306</v>
       </c>
       <c r="Q18" t="n">
-        <v>153.4308348336508</v>
+        <v>135.0709875386965</v>
       </c>
     </row>
     <row r="19">
@@ -1457,52 +1457,52 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>0.9999999997629182</v>
+        <v>0.9994428270871609</v>
       </c>
       <c r="C19" t="n">
-        <v>-0.6096389565638431</v>
+        <v>0.7044114657269106</v>
       </c>
       <c r="D19" t="n">
-        <v>0.999999996350974</v>
+        <v>0.9977590370709437</v>
       </c>
       <c r="E19" t="n">
-        <v>0.9999999003775992</v>
+        <v>0.9980221834685008</v>
       </c>
       <c r="F19" t="n">
-        <v>0.9999999892981991</v>
+        <v>0.9980974571392236</v>
       </c>
       <c r="G19" t="n">
-        <v>3.505965994382825e-08</v>
+        <v>0.0003307619096778958</v>
       </c>
       <c r="H19" t="n">
-        <v>238.0334588651932</v>
+        <v>0.1754741227043277</v>
       </c>
       <c r="I19" t="n">
-        <v>6.469692111507101e-08</v>
+        <v>0.001351741718049761</v>
       </c>
       <c r="J19" t="n">
-        <v>1.5284359946659e-07</v>
+        <v>0.0004350831228328726</v>
       </c>
       <c r="K19" t="n">
-        <v>1.087702602908305e-07</v>
+        <v>0.0008934124204413166</v>
       </c>
       <c r="L19" t="n">
-        <v>0.0001009418757217764</v>
+        <v>0.007308309815769336</v>
       </c>
       <c r="M19" t="n">
-        <v>0.0001872422493558231</v>
+        <v>0.01818686090775139</v>
       </c>
       <c r="N19" t="n">
-        <v>1.000000000437689</v>
+        <v>1.001028626916011</v>
       </c>
       <c r="O19" t="n">
-        <v>0.0001952135395557907</v>
+        <v>0.0189611132285865</v>
       </c>
       <c r="P19" t="n">
-        <v>108.3324293135273</v>
+        <v>90.0282234950421</v>
       </c>
       <c r="Q19" t="n">
-        <v>153.4308348336508</v>
+        <v>135.1266290151655</v>
       </c>
     </row>
     <row r="20">
@@ -1512,52 +1512,52 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>0.9999999997629182</v>
+        <v>0.9994541085875467</v>
       </c>
       <c r="C20" t="n">
-        <v>-0.6096389565638431</v>
+        <v>0.7042012905996862</v>
       </c>
       <c r="D20" t="n">
-        <v>0.999999996350974</v>
+        <v>0.9977561486508768</v>
       </c>
       <c r="E20" t="n">
-        <v>0.9999999003775992</v>
+        <v>0.9979779440560075</v>
       </c>
       <c r="F20" t="n">
-        <v>0.9999999892981991</v>
+        <v>0.9980852399132882</v>
       </c>
       <c r="G20" t="n">
-        <v>3.505965994382825e-08</v>
+        <v>0.0003240647237134707</v>
       </c>
       <c r="H20" t="n">
-        <v>238.0334588651932</v>
+        <v>0.1755988917389408</v>
       </c>
       <c r="I20" t="n">
-        <v>6.469692111507101e-08</v>
+        <v>0.001353484003856029</v>
       </c>
       <c r="J20" t="n">
-        <v>1.5284359946659e-07</v>
+        <v>0.0004448149768412178</v>
       </c>
       <c r="K20" t="n">
-        <v>1.087702602908305e-07</v>
+        <v>0.0008991494903486234</v>
       </c>
       <c r="L20" t="n">
-        <v>0.0001009418757217764</v>
+        <v>0.006903125591599197</v>
       </c>
       <c r="M20" t="n">
-        <v>0.0001872422493558231</v>
+        <v>0.01800179779115049</v>
       </c>
       <c r="N20" t="n">
-        <v>1.000000000437689</v>
+        <v>1.001007799530683</v>
       </c>
       <c r="O20" t="n">
-        <v>0.0001952135395557907</v>
+        <v>0.01876817159197844</v>
       </c>
       <c r="P20" t="n">
-        <v>108.3324293135273</v>
+        <v>90.06913459514895</v>
       </c>
       <c r="Q20" t="n">
-        <v>153.4308348336508</v>
+        <v>135.1675401152724</v>
       </c>
     </row>
     <row r="21">
@@ -1567,52 +1567,52 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>0.9999999997629182</v>
+        <v>0.9994619605346218</v>
       </c>
       <c r="C21" t="n">
-        <v>-0.6096389565638431</v>
+        <v>0.7040084668431268</v>
       </c>
       <c r="D21" t="n">
-        <v>0.999999996350974</v>
+        <v>0.9977512239613215</v>
       </c>
       <c r="E21" t="n">
-        <v>0.9999999003775992</v>
+        <v>0.9979274818162044</v>
       </c>
       <c r="F21" t="n">
-        <v>0.9999999892981991</v>
+        <v>0.9980702573109567</v>
       </c>
       <c r="G21" t="n">
-        <v>3.505965994382825e-08</v>
+        <v>0.0003194034687432521</v>
       </c>
       <c r="H21" t="n">
-        <v>238.0334588651932</v>
+        <v>0.175713360250387</v>
       </c>
       <c r="I21" t="n">
-        <v>6.469692111507101e-08</v>
+        <v>0.00135645456094734</v>
       </c>
       <c r="J21" t="n">
-        <v>1.5284359946659e-07</v>
+        <v>0.0004559157379730189</v>
       </c>
       <c r="K21" t="n">
-        <v>1.087702602908305e-07</v>
+        <v>0.0009061851494601796</v>
       </c>
       <c r="L21" t="n">
-        <v>0.0001009418757217764</v>
+        <v>0.006601960641642268</v>
       </c>
       <c r="M21" t="n">
-        <v>0.0001872422493558231</v>
+        <v>0.01787186248669265</v>
       </c>
       <c r="N21" t="n">
-        <v>1.000000000437689</v>
+        <v>1.000993303628391</v>
       </c>
       <c r="O21" t="n">
-        <v>0.0001952135395557907</v>
+        <v>0.01863270467260667</v>
       </c>
       <c r="P21" t="n">
-        <v>108.3324293135273</v>
+        <v>90.09811092411364</v>
       </c>
       <c r="Q21" t="n">
-        <v>153.4308348336508</v>
+        <v>135.1965164442371</v>
       </c>
     </row>
     <row r="22">
@@ -1622,52 +1622,52 @@
         </is>
       </c>
       <c r="B22" t="n">
-        <v>0.9999999997629182</v>
+        <v>0.9994671610884248</v>
       </c>
       <c r="C22" t="n">
-        <v>-0.6096389565638431</v>
+        <v>0.703832040289722</v>
       </c>
       <c r="D22" t="n">
-        <v>0.999999996350974</v>
+        <v>0.9977449153517669</v>
       </c>
       <c r="E22" t="n">
-        <v>0.9999999003775992</v>
+        <v>0.9978735515126238</v>
       </c>
       <c r="F22" t="n">
-        <v>0.9999999892981991</v>
+        <v>0.9980535735534197</v>
       </c>
       <c r="G22" t="n">
-        <v>3.505965994382825e-08</v>
+        <v>0.0003163161953534975</v>
       </c>
       <c r="H22" t="n">
-        <v>238.0334588651932</v>
+        <v>0.1758180946737184</v>
       </c>
       <c r="I22" t="n">
-        <v>6.469692111507101e-08</v>
+        <v>0.001360259894184849</v>
       </c>
       <c r="J22" t="n">
-        <v>1.5284359946659e-07</v>
+        <v>0.0004677794091090777</v>
       </c>
       <c r="K22" t="n">
-        <v>1.087702602908305e-07</v>
+        <v>0.0009140196516469632</v>
       </c>
       <c r="L22" t="n">
-        <v>0.0001009418757217764</v>
+        <v>0.006332536211601226</v>
       </c>
       <c r="M22" t="n">
-        <v>0.0001872422493558231</v>
+        <v>0.01778528030011047</v>
       </c>
       <c r="N22" t="n">
-        <v>1.000000000437689</v>
+        <v>1.000983702605985</v>
       </c>
       <c r="O22" t="n">
-        <v>0.0001952135395557907</v>
+        <v>0.01854243650309184</v>
       </c>
       <c r="P22" t="n">
-        <v>108.3324293135273</v>
+        <v>90.11753645290958</v>
       </c>
       <c r="Q22" t="n">
-        <v>153.4308348336508</v>
+        <v>135.215941973033</v>
       </c>
     </row>
     <row r="23">
@@ -1677,52 +1677,52 @@
         </is>
       </c>
       <c r="B23" t="n">
-        <v>0.9999999997629182</v>
+        <v>0.9994703415779579</v>
       </c>
       <c r="C23" t="n">
-        <v>-0.6096389565638431</v>
+        <v>0.7036707385103448</v>
       </c>
       <c r="D23" t="n">
-        <v>0.999999996350974</v>
+        <v>0.9977377550850697</v>
       </c>
       <c r="E23" t="n">
-        <v>0.9999999003775992</v>
+        <v>0.9978180314709649</v>
       </c>
       <c r="F23" t="n">
-        <v>0.9999999892981991</v>
+        <v>0.9980359704486846</v>
       </c>
       <c r="G23" t="n">
-        <v>3.505965994382825e-08</v>
+        <v>0.0003144281193767107</v>
       </c>
       <c r="H23" t="n">
-        <v>238.0334588651932</v>
+        <v>0.1759138503778308</v>
       </c>
       <c r="I23" t="n">
-        <v>6.469692111507101e-08</v>
+        <v>0.001364578944304522</v>
       </c>
       <c r="J23" t="n">
-        <v>1.5284359946659e-07</v>
+        <v>0.0004799927932728892</v>
       </c>
       <c r="K23" t="n">
-        <v>1.087702602908305e-07</v>
+        <v>0.0009222858687887056</v>
       </c>
       <c r="L23" t="n">
-        <v>0.0001009418757217764</v>
+        <v>0.006089985002528078</v>
       </c>
       <c r="M23" t="n">
-        <v>0.0001872422493558231</v>
+        <v>0.01773212111893867</v>
       </c>
       <c r="N23" t="n">
-        <v>1.000000000437689</v>
+        <v>1.000977830933001</v>
       </c>
       <c r="O23" t="n">
-        <v>0.0001952135395557907</v>
+        <v>0.01848701422552288</v>
       </c>
       <c r="P23" t="n">
-        <v>108.3324293135273</v>
+        <v>90.12951012637498</v>
       </c>
       <c r="Q23" t="n">
-        <v>153.4308348336508</v>
+        <v>135.2279156464984</v>
       </c>
     </row>
     <row r="24">
@@ -1732,52 +1732,52 @@
         </is>
       </c>
       <c r="B24" t="n">
-        <v>0.9999999997629182</v>
+        <v>0.9994719697574035</v>
       </c>
       <c r="C24" t="n">
-        <v>-0.6096389565638431</v>
+        <v>0.7035235158185215</v>
       </c>
       <c r="D24" t="n">
-        <v>0.999999996350974</v>
+        <v>0.9977300670574192</v>
       </c>
       <c r="E24" t="n">
-        <v>0.9999999003775992</v>
+        <v>0.9977623510930335</v>
       </c>
       <c r="F24" t="n">
-        <v>0.9999999892981991</v>
+        <v>0.9980179916904994</v>
       </c>
       <c r="G24" t="n">
-        <v>3.505965994382825e-08</v>
+        <v>0.0003134615617241146</v>
       </c>
       <c r="H24" t="n">
-        <v>238.0334588651932</v>
+        <v>0.1760012481273863</v>
       </c>
       <c r="I24" t="n">
-        <v>6.469692111507101e-08</v>
+        <v>0.001369216338154251</v>
       </c>
       <c r="J24" t="n">
-        <v>1.5284359946659e-07</v>
+        <v>0.0004922414484565769</v>
       </c>
       <c r="K24" t="n">
-        <v>1.087702602908305e-07</v>
+        <v>0.0009307284885046045</v>
       </c>
       <c r="L24" t="n">
-        <v>0.0001009418757217764</v>
+        <v>0.0058716599726902</v>
       </c>
       <c r="M24" t="n">
-        <v>0.0001872422493558231</v>
+        <v>0.01770484571308416</v>
       </c>
       <c r="N24" t="n">
-        <v>1.000000000437689</v>
+        <v>1.000974825063255</v>
       </c>
       <c r="O24" t="n">
-        <v>0.0001952135395557907</v>
+        <v>0.01845857764917328</v>
       </c>
       <c r="P24" t="n">
-        <v>108.3324293135273</v>
+        <v>90.13566763107789</v>
       </c>
       <c r="Q24" t="n">
-        <v>153.4308348336508</v>
+        <v>135.2340731512013</v>
       </c>
     </row>
     <row r="25">
@@ -1787,52 +1787,52 @@
         </is>
       </c>
       <c r="B25" t="n">
-        <v>0.9999999997629182</v>
+        <v>0.9994724538681431</v>
       </c>
       <c r="C25" t="n">
-        <v>-0.6096389565638431</v>
+        <v>0.7033893620835143</v>
       </c>
       <c r="D25" t="n">
-        <v>0.999999996350974</v>
+        <v>0.9977221760679598</v>
       </c>
       <c r="E25" t="n">
-        <v>0.9999999003775992</v>
+        <v>0.9977076914777816</v>
       </c>
       <c r="F25" t="n">
-        <v>0.9999999892981991</v>
+        <v>0.9980001199449472</v>
       </c>
       <c r="G25" t="n">
-        <v>3.505965994382825e-08</v>
+        <v>0.0003131741726765522</v>
       </c>
       <c r="H25" t="n">
-        <v>238.0334588651932</v>
+        <v>0.1760808875796261</v>
       </c>
       <c r="I25" t="n">
-        <v>6.469692111507101e-08</v>
+        <v>0.001373976157922198</v>
       </c>
       <c r="J25" t="n">
-        <v>1.5284359946659e-07</v>
+        <v>0.0005042655546958971</v>
       </c>
       <c r="K25" t="n">
-        <v>1.087702602908305e-07</v>
+        <v>0.0009391208563090476</v>
       </c>
       <c r="L25" t="n">
-        <v>0.0001009418757217764</v>
+        <v>0.005675224531835206</v>
       </c>
       <c r="M25" t="n">
-        <v>0.0001872422493558231</v>
+        <v>0.01769672773923338</v>
       </c>
       <c r="N25" t="n">
-        <v>1.000000000437689</v>
+        <v>1.000973931320351</v>
       </c>
       <c r="O25" t="n">
-        <v>0.0001952135395557907</v>
+        <v>0.01845011407636915</v>
       </c>
       <c r="P25" t="n">
-        <v>108.3324293135273</v>
+        <v>90.1375021199328</v>
       </c>
       <c r="Q25" t="n">
-        <v>153.4308348336508</v>
+        <v>135.2359076400562</v>
       </c>
     </row>
     <row r="26">
@@ -1842,52 +1842,52 @@
         </is>
       </c>
       <c r="B26" t="n">
-        <v>0.9999999997629182</v>
+        <v>0.9994720869335167</v>
       </c>
       <c r="C26" t="n">
-        <v>-0.6096389565638431</v>
+        <v>0.7032670492476716</v>
       </c>
       <c r="D26" t="n">
-        <v>0.999999996350974</v>
+        <v>0.9977143537634454</v>
       </c>
       <c r="E26" t="n">
-        <v>0.9999999003775992</v>
+        <v>0.9976546453218683</v>
       </c>
       <c r="F26" t="n">
-        <v>0.9999999892981991</v>
+        <v>0.9979826710923455</v>
       </c>
       <c r="G26" t="n">
-        <v>3.505965994382825e-08</v>
+        <v>0.0003133920009215122</v>
       </c>
       <c r="H26" t="n">
-        <v>238.0334588651932</v>
+        <v>0.1761534977626218</v>
       </c>
       <c r="I26" t="n">
-        <v>6.469692111507101e-08</v>
+        <v>0.001378694547149585</v>
       </c>
       <c r="J26" t="n">
-        <v>1.5284359946659e-07</v>
+        <v>0.0005159347296681419</v>
       </c>
       <c r="K26" t="n">
-        <v>1.087702602908305e-07</v>
+        <v>0.0009473146384088635</v>
       </c>
       <c r="L26" t="n">
-        <v>0.0001009418757217764</v>
+        <v>0.005498478620867583</v>
       </c>
       <c r="M26" t="n">
-        <v>0.0001872422493558231</v>
+        <v>0.01770288114747179</v>
       </c>
       <c r="N26" t="n">
-        <v>1.000000000437689</v>
+        <v>1.000974608738123</v>
       </c>
       <c r="O26" t="n">
-        <v>0.0001952135395557907</v>
+        <v>0.01845652944793558</v>
       </c>
       <c r="P26" t="n">
-        <v>108.3324293135273</v>
+        <v>90.13611150382289</v>
       </c>
       <c r="Q26" t="n">
-        <v>153.4308348336508</v>
+        <v>135.2345170239463</v>
       </c>
     </row>
   </sheetData>

</xml_diff>